<commit_message>
Add examples of xlsx files
</commit_message>
<xml_diff>
--- a/SpreadsheetSerializer.Tests.Unit/DataSource1/ExampleWorkbook.xlsx
+++ b/SpreadsheetSerializer.Tests.Unit/DataSource1/ExampleWorkbook.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" activeTab="0"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId2"/>
     <sheet name="UserSettings" sheetId="3" r:id="rId3"/>
+    <sheet name="Evaluation Warning" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr fullCalcOnLoad="1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>Id</t>
   </si>
@@ -70,16 +71,27 @@
   </si>
   <si>
     <t>150%</t>
+  </si>
+  <si>
+    <t>Evaluation Only. Created with Aspose.Cells for .NET.Copyright 2003 - 2020 Aspose Pty Ltd.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="18"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -126,8 +138,12 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment/>
+      <protection/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,7 +520,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xr:uid="{e75d1c2a-2801-4d7a-9776-7175185666db}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xr:uid="{4e62c41e-1b1d-44a3-bbb2-9d9bacf3f836}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1"/>
@@ -556,7 +572,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xr:uid="{43871584-5a55-43ee-88a1-c1be78a6b5c6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xr:uid="{2aed0c89-8385-4f63-88f2-e715a43f6b8d}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1"/>
@@ -629,4 +645,23 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xr:uid="{fad6c089-28cd-4bd6-9f17-421a24d056af}">
+  <dimension ref="A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="5" spans="1:1" ht="23.25" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
clean code an rerun all unit tests
</commit_message>
<xml_diff>
--- a/SpreadsheetSerializer.Tests.Unit/DataSource1/ExampleWorkbook.xlsx
+++ b/SpreadsheetSerializer.Tests.Unit/DataSource1/ExampleWorkbook.xlsx
@@ -520,7 +520,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xr:uid="{e076a9a6-fea2-4977-8e22-3bf2617ba7c5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xr:uid="{0d1461ec-cc09-436c-bfef-c1aa1c5d32af}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1"/>
@@ -572,7 +572,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xr:uid="{d2bda9da-352c-4391-a7c5-c4b95aa82e66}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xr:uid="{7f53ac52-76c6-4a9a-85e3-97d63f72f8e7}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1"/>
@@ -648,7 +648,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xr:uid="{f47f146f-cc91-467a-87b7-950f91c29a2d}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xr:uid="{1cfc8608-f6f6-4c54-b381-4edce34c8f30}">
   <dimension ref="A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>

</xml_diff>